<commit_message>
developed function to split id-yr into nesting attempts, and working on changepoint analyses
</commit_message>
<xml_diff>
--- a/fieldNotes/Argos_posthatch.xlsx
+++ b/fieldNotes/Argos_posthatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive\Desktop\nestAutoEval\fieldNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14064\Desktop\nestAutoEval\fieldNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DF3C3BA-6774-422C-82A3-980D5AEF80C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3492B70-E026-49E5-B37C-4821BC8333B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="4665" windowWidth="24240" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12930" yWindow="-16320" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LatestDayAdultSeenChickGuiding" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="FirstDayFledgedChickSeen" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -902,16 +901,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +927,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -945,7 +944,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -959,7 +958,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -973,7 +972,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -987,7 +986,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
@@ -1008,17 +1007,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1089,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="s">
         <v>30</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
@@ -1533,7 +1532,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A23" s="12" t="s">
         <v>23</v>
       </c>
@@ -1556,7 +1555,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A24" s="12" t="s">
         <v>25</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A25" s="12" t="s">
         <v>32</v>
       </c>
@@ -1602,7 +1601,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A26" s="12" t="s">
         <v>5</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A27" s="12" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A28" s="12" t="s">
         <v>12</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A29" s="12" t="s">
         <v>13</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A30" s="12" t="s">
         <v>25</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A31" s="12" t="s">
         <v>33</v>
       </c>
@@ -1751,17 +1750,19 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.31640625" customWidth="1"/>
+    <col min="2" max="2" width="24.953125" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.76953125" customWidth="1"/>
+    <col min="5" max="5" width="17.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>

</xml_diff>